<commit_message>
* implement all cell parsers (simple literal and uri, multi line literal and uri and simple and multi line commented values)
* implement columns creation from legal document property worksheet
</commit_message>
<xml_diff>
--- a/docs/semi-structured/LAM_metadata_03.xlsx
+++ b/docs/semi-structured/LAM_metadata_03.xlsx
@@ -5,13 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LAM metadata" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Classes complete" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="CELEX metadata" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="CELEX classes" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="prefixes" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3482" uniqueCount="905">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3542" uniqueCount="963">
   <si>
     <t xml:space="preserve">URI</t>
   </si>
@@ -3280,6 +3281,180 @@
   <si>
     <t xml:space="preserve">CB</t>
   </si>
+  <si>
+    <t xml:space="preserve">prefix</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">evo:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://eurovoc.europa.eu/schema#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skos:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.w3.org/2004/02/skos/core#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skoxl:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.w3.org/2008/05/skos-xl#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdf:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.w3.org/1999/02/22-rdf-syntax-ns#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">xsd:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.w3.org/2001/XMLSchema#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rdfs:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.w3.org/2000/01/rdf-schema#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dct:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.org/dc/terms/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dc:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://purl.org/dc/elements/1.1/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">owl:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.w3.org/2002/07/owl#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">euvoc:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://publications.europa.eu/ontology/euvoc#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vb:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://art.uniroma2.it/ontologies/vocbench#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lexvo:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://lexvo.org/ontology#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lemon:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://lemon-model.net/lemon#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">void:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://rdfs.org/ns/void#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ato:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://publications.europa.eu/ontology/authority/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">atr:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://publications.europa.eu/resource/authority/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">atdt:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://publications.europa.eu/ontology/datatype#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">atmdr:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://publications.europa.eu/mdr/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">geowgs:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.w3.org/2003/01/geo/wgs84_pos#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">org:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.w3.org/ns/org#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">foaf:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://xmlns.com/foaf/0.1/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lam:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://publications.europa.eu/ontology/lam-skos-ap#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ann</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://publications.europa.eu/ontology/annotation#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lamd:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://publications.europa.eu/resources/authority/lam/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cdm:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://publications.europa.eu/ontology/cdm#</t>
+  </si>
+  <si>
+    <t xml:space="preserve">at:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fd:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">celexd:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://publications.europa.eu/resources/authority/celex/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sh:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.w3.org/ns/shacl#</t>
+  </si>
 </sst>
 </file>
 
@@ -3288,7 +3463,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3316,6 +3491,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -3393,7 +3574,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3414,16 +3595,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -3507,10 +3692,10 @@
   </sheetPr>
   <dimension ref="A1:AB107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="X1" activeCellId="0" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="X9" activeCellId="0" sqref="X9"/>
+      <selection pane="bottomLeft" activeCell="X9" activeCellId="1" sqref="A1:B33 X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7669,7 +7854,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CN1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="CN1" activeCellId="0" sqref="CN1"/>
-      <selection pane="bottomLeft" activeCell="CP1" activeCellId="0" sqref="CP1"/>
+      <selection pane="bottomLeft" activeCell="CP1" activeCellId="1" sqref="A1:B33 CP1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7677,7 +7862,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="10.9"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="61.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="8.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="19.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="19.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="155.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="22.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="31.09"/>
@@ -7721,14 +7906,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="46" min="46" style="3" width="3.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="47" min="47" style="3" width="3.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="48" min="48" style="3" width="3.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="11.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="49" min="49" style="3" width="11.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="50" min="50" style="3" width="9.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="51" min="51" style="3" width="7.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="3" width="11.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="3" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="3" width="13.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="3" width="17.05"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="3" width="11.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="3" width="17.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="3" width="11.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="3" width="12.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="3" width="13.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="59" min="59" style="3" width="13.81"/>
@@ -7739,7 +7924,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="64" style="3" width="14.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="65" min="65" style="3" width="15.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="66" min="66" style="3" width="8.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="3" width="8.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="67" min="67" style="3" width="8.94"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="68" min="68" style="3" width="12.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="69" style="3" width="17.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="70" min="70" style="3" width="14.62"/>
@@ -13850,7 +14035,7 @@
   <dimension ref="A1:AB8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB2" activeCellId="0" sqref="AB2"/>
+      <selection pane="topLeft" activeCell="AB2" activeCellId="1" sqref="A1:B33 AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14147,7 +14332,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="1" sqref="A1:B33 J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14517,4 +14702,274 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B31"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="9.14"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>905</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>906</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>907</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>909</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>910</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>911</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>913</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>914</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>915</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>916</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>917</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>919</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>920</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>921</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>922</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>923</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>924</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>925</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>927</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>928</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>929</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>930</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>931</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>933</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>934</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>935</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>936</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>937</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>939</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="s">
+        <v>941</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>942</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="s">
+        <v>943</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>944</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>945</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>946</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>947</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>948</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>949</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>950</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>951</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>952</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="s">
+        <v>953</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>954</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>955</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>956</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>957</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>958</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>938</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>959</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>961</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>962</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
* implement multi column triple maker - very versatile result * implement triple pattern maker - flexible easy to use, handy for reification * TODO: clean up old code, remove plain triple maker and the column triple maker
</commit_message>
<xml_diff>
--- a/docs/semi-structured/LAM_metadata_03.xlsx
+++ b/docs/semi-structured/LAM_metadata_03.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="LAM metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3542" uniqueCount="963">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3543" uniqueCount="963">
   <si>
     <t xml:space="preserve">URI</t>
   </si>
@@ -1925,8 +1925,8 @@
     <t xml:space="preserve">cdm:communication_cjeu_has_type_procedure_concept_type_procedure</t>
   </si>
   <si>
-    <t xml:space="preserve">at:legal proceeding
-at:legal proceeding_result
+    <t xml:space="preserve">at:legal_proceeding
+at:legal_proceeding_result
 fd:fd_110</t>
   </si>
   <si>
@@ -3288,6 +3288,9 @@
     <t xml:space="preserve">uri</t>
   </si>
   <si>
+    <t xml:space="preserve">http://publications.europa.eu/resources/authority/lam/</t>
+  </si>
+  <si>
     <t xml:space="preserve">evo:</t>
   </si>
   <si>
@@ -3427,9 +3430,6 @@
   </si>
   <si>
     <t xml:space="preserve">lamd:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://publications.europa.eu/resources/authority/lam/</t>
   </si>
   <si>
     <t xml:space="preserve">cdm:</t>
@@ -3463,7 +3463,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3491,12 +3491,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -3574,7 +3568,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3605,10 +3599,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -3692,10 +3682,10 @@
   </sheetPr>
   <dimension ref="A1:AB107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="X1" activeCellId="0" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="X9" activeCellId="1" sqref="A1:B33 X9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="E83" activeCellId="0" sqref="E83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6904,7 +6894,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="83" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="83" customFormat="false" ht="41.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="0" t="s">
         <v>497</v>
       </c>
@@ -7854,7 +7844,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CN1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="CN1" activeCellId="0" sqref="CN1"/>
-      <selection pane="bottomLeft" activeCell="CP1" activeCellId="1" sqref="A1:B33 CP1"/>
+      <selection pane="bottomLeft" activeCell="CP1" activeCellId="0" sqref="CP1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14035,7 +14025,7 @@
   <dimension ref="A1:AB8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB2" activeCellId="1" sqref="A1:B33 AB2"/>
+      <selection pane="topLeft" activeCell="AB2" activeCellId="0" sqref="AB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14332,7 +14322,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="1" sqref="A1:B33 J2"/>
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14709,10 +14699,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B31"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:B33"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14729,240 +14719,245 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>907</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>908</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>908</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>909</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>910</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>910</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>911</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>912</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>912</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>913</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>914</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>914</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>915</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>916</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>916</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>917</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>918</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>918</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>919</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>920</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>920</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>921</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>922</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>922</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>923</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>924</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>924</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>925</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>926</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>926</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>927</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>928</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>928</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>929</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>930</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>930</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>931</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>932</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>932</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>933</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>934</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>934</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>935</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>936</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>936</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>937</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>938</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>938</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>939</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>940</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>940</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>941</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>942</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>942</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>943</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>944</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>944</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>945</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>946</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>946</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>947</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>948</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>948</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>949</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>950</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>950</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>951</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>952</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>952</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>953</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>954</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>956</v>
+        <v>907</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>957</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>938</v>
+        <v>955</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>956</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>958</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>938</v>
+        <v>957</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>939</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>959</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>960</v>
+        <v>958</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>939</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>959</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>960</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
         <v>961</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B31" s="1" t="s">
         <v>962</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
* implement property worksheet generation * start implementing lam class worksheet
</commit_message>
<xml_diff>
--- a/docs/semi-structured/LAM_metadata_03.xlsx
+++ b/docs/semi-structured/LAM_metadata_03.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LAM metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3543" uniqueCount="963">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3533" uniqueCount="962">
   <si>
     <t xml:space="preserve">URI</t>
   </si>
@@ -44,7 +44,7 @@
     <t xml:space="preserve">annotation_1</t>
   </si>
   <si>
-    <t xml:space="preserve">controlled value_annotation_1 </t>
+    <t xml:space="preserve">controlled value_annotation_1</t>
   </si>
   <si>
     <t xml:space="preserve">annotation_2</t>
@@ -2354,7 +2354,7 @@
     <t xml:space="preserve">YU</t>
   </si>
   <si>
-    <t xml:space="preserve">5*XC_OJC</t>
+    <t xml:space="preserve">celexd:5_XC_OJC</t>
   </si>
   <si>
     <t xml:space="preserve">N</t>
@@ -2486,7 +2486,7 @@
     <t xml:space="preserve">OPIN_EXPLOR</t>
   </si>
   <si>
-    <t xml:space="preserve">5*AE</t>
+    <t xml:space="preserve">celexd:5_AE</t>
   </si>
   <si>
     <t xml:space="preserve">fd:fd_365/DATVOT</t>
@@ -2596,7 +2596,7 @@
     <t xml:space="preserve">OWNINI_OPIN</t>
   </si>
   <si>
-    <t xml:space="preserve">5*IE</t>
+    <t xml:space="preserve">celexd:5_IE</t>
   </si>
   <si>
     <t xml:space="preserve">lamd:c_009</t>
@@ -2646,7 +2646,7 @@
     <t xml:space="preserve">STAT_REASON</t>
   </si>
   <si>
-    <t xml:space="preserve">5*AG</t>
+    <t xml:space="preserve">celexd:5_AG</t>
   </si>
   <si>
     <t xml:space="preserve">N| Currently, there is 9999 used with annotation Linked to proposal, but the date is not updated.</t>
@@ -2684,7 +2684,7 @@
     <t xml:space="preserve">PROP_REG</t>
   </si>
   <si>
-    <t xml:space="preserve">5*PC_EUR</t>
+    <t xml:space="preserve">celexd:5_PC_EUR</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -2867,7 +2867,7 @@
     <t xml:space="preserve">INFO_JUDICIAL</t>
   </si>
   <si>
-    <t xml:space="preserve">6*CA</t>
+    <t xml:space="preserve">celexd:6_CA</t>
   </si>
   <si>
     <t xml:space="preserve">Y| link to judgment 6*CJ</t>
@@ -2895,7 +2895,7 @@
     <t xml:space="preserve">62018CB0373</t>
   </si>
   <si>
-    <t xml:space="preserve">6*CB</t>
+    <t xml:space="preserve">celexd:6_CB</t>
   </si>
   <si>
     <t xml:space="preserve">Y| link to order 6*CO</t>
@@ -2926,7 +2926,7 @@
     <t xml:space="preserve">ARRANG</t>
   </si>
   <si>
-    <t xml:space="preserve">2*A_OJL</t>
+    <t xml:space="preserve">celexd:2_A_OJL</t>
   </si>
   <si>
     <t xml:space="preserve">fd:fd_365/DATSIG</t>
@@ -2979,6 +2979,9 @@
   </si>
   <si>
     <t xml:space="preserve">Withdrawals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">controlled value_annotation_1 </t>
   </si>
   <si>
     <t xml:space="preserve">celexd:md_001</t>
@@ -3127,7 +3130,7 @@
     <t xml:space="preserve">CELEX_ID</t>
   </si>
   <si>
-    <t xml:space="preserve">celexd:c_001</t>
+    <t xml:space="preserve">2_A_OJL</t>
   </si>
   <si>
     <t xml:space="preserve">Agreements with Member or non-member States  or international organisations</t>
@@ -3145,10 +3148,7 @@
     <t xml:space="preserve">??</t>
   </si>
   <si>
-    <t xml:space="preserve">celexd:c_002</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2*A_OJC</t>
+    <t xml:space="preserve">2_A_OJC</t>
   </si>
   <si>
     <t xml:space="preserve">22012A1013(01): Monetary Agreement between the European Union and the Principality of Monaco</t>
@@ -3157,10 +3157,7 @@
     <t xml:space="preserve">Last publication in OJ-C in 2012</t>
   </si>
   <si>
-    <t xml:space="preserve">celexd:c_003</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5*XC_OJL</t>
+    <t xml:space="preserve">5_XC_OJL</t>
   </si>
   <si>
     <t xml:space="preserve">Other documents of the Commission OJ-L</t>
@@ -3172,7 +3169,7 @@
     <t xml:space="preserve">XC</t>
   </si>
   <si>
-    <t xml:space="preserve">celexd:c_004</t>
+    <t xml:space="preserve">5_XC_OJC</t>
   </si>
   <si>
     <t xml:space="preserve">Other documents of the Commission OJ-C</t>
@@ -3181,7 +3178,7 @@
     <t xml:space="preserve">52014XC1205(01): Authorisation for State aid pursuant to Articles 107 and 108 of the Treaty on the Functioning of the European Union — Cases where the Commission raises no objections Text with EEA relevance</t>
   </si>
   <si>
-    <t xml:space="preserve">celexd:c_005</t>
+    <t xml:space="preserve">5_AE</t>
   </si>
   <si>
     <t xml:space="preserve">Opinions on consultation of the European Economic and Social Committee</t>
@@ -3199,7 +3196,7 @@
     <t xml:space="preserve">Internal number | EESC-2014-01723-00-00-AC-TRA: it is not mentioned in the Official Journal. It can be found on ECSC web page.</t>
   </si>
   <si>
-    <t xml:space="preserve">celexd:c_006</t>
+    <t xml:space="preserve">5_IE</t>
   </si>
   <si>
     <t xml:space="preserve">Own-initiative opinions of the European Economic and Social Committee </t>
@@ -3211,7 +3208,7 @@
     <t xml:space="preserve">IE</t>
   </si>
   <si>
-    <t xml:space="preserve">celexd:c_007</t>
+    <t xml:space="preserve">5_AG</t>
   </si>
   <si>
     <t xml:space="preserve">5*AG Council positions and statement of reasons</t>
@@ -3233,7 +3230,7 @@
     <t xml:space="preserve">Official No (PPF)| There is a split number – (01) for position of the Council, (02) for statement of Council´s reasons.</t>
   </si>
   <si>
-    <t xml:space="preserve">celexd:c_008</t>
+    <t xml:space="preserve">5_PC_EUR</t>
   </si>
   <si>
     <t xml:space="preserve">COM - legislative proposals, and documents related</t>
@@ -3252,7 +3249,7 @@
     <t xml:space="preserve">COM number</t>
   </si>
   <si>
-    <t xml:space="preserve">celexd:c_009</t>
+    <t xml:space="preserve">6_CA</t>
   </si>
   <si>
     <t xml:space="preserve">Judicial information: Judgment</t>
@@ -3270,7 +3267,7 @@
     <t xml:space="preserve">Case number</t>
   </si>
   <si>
-    <t xml:space="preserve">celexd:c_010</t>
+    <t xml:space="preserve">6_CB</t>
   </si>
   <si>
     <t xml:space="preserve">Judicial information: Order</t>
@@ -3303,7 +3300,7 @@
     <t xml:space="preserve">http://www.w3.org/2004/02/skos/core#</t>
   </si>
   <si>
-    <t xml:space="preserve">skoxl:</t>
+    <t xml:space="preserve">skosxl:</t>
   </si>
   <si>
     <t xml:space="preserve">http://www.w3.org/2008/05/skos-xl#</t>
@@ -3682,10 +3679,10 @@
   </sheetPr>
   <dimension ref="A1:AB107"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="E83" activeCellId="0" sqref="E83"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B93" activeCellId="0" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7841,10 +7838,10 @@
   </sheetPr>
   <dimension ref="A1:CR21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="CN1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="CN1" activeCellId="0" sqref="CN1"/>
-      <selection pane="bottomLeft" activeCell="CP1" activeCellId="0" sqref="CP1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="K23" activeCellId="0" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7859,7 +7856,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="29.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="18.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="3.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="9.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="16.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="9.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="21.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="20.88"/>
@@ -14058,7 +14055,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>6</v>
+        <v>815</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
@@ -14126,25 +14123,25 @@
     </row>
     <row r="2" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="Z2" s="0" t="s">
         <v>72</v>
@@ -14158,22 +14155,22 @@
     </row>
     <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="Z3" s="0" t="s">
         <v>72</v>
@@ -14187,25 +14184,25 @@
     </row>
     <row r="4" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="U4" s="0" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="Z4" s="0" t="s">
         <v>72</v>
@@ -14219,25 +14216,25 @@
     </row>
     <row r="5" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="U5" s="0" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="Z5" s="0" t="s">
         <v>72</v>
@@ -14251,7 +14248,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>29</v>
@@ -14265,7 +14262,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>33</v>
@@ -14274,33 +14271,33 @@
         <v>34</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="U8" s="0" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="Z8" s="0" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="AA8" s="0" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
     </row>
   </sheetData>
@@ -14322,7 +14319,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14357,59 +14354,61 @@
         <v>50</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>854</v>
+      <c r="A2" s="0" t="str">
+        <f aca="false">CONCATENATE("celexd:",B2)</f>
+        <v>celexd:2_A_OJL</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>797</v>
+        <v>855</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>2</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>860</v>
+      <c r="A3" s="0" t="str">
+        <f aca="false">CONCATENATE("celexd:",B3)</f>
+        <v>celexd:2_A_OJC</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>861</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="D3" s="0" t="s">
         <v>862</v>
@@ -14421,266 +14420,274 @@
         <v>2</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="0" t="str">
+        <f aca="false">CONCATENATE("celexd:",B4)</f>
+        <v>celexd:5_XC_OJL</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>864</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="C4" s="0" t="s">
         <v>865</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>866</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>867</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G4" s="0" t="s">
+        <v>867</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>859</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>859</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="str">
+        <f aca="false">CONCATENATE("celexd:",B5)</f>
+        <v>celexd:5_XC_OJC</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>868</v>
       </c>
-      <c r="H4" s="0" t="s">
-        <v>858</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>858</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="C5" s="0" t="s">
         <v>869</v>
       </c>
-      <c r="B5" s="0" t="s">
-        <v>634</v>
-      </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>870</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>871</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="0" t="str">
+        <f aca="false">CONCATENATE("celexd:",B6)</f>
+        <v>celexd:5_AE</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>871</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>872</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>675</v>
-      </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>873</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="E6" s="0" t="s">
         <v>874</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>875</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G6" s="0" t="s">
+        <v>875</v>
+      </c>
+      <c r="H6" s="0" t="s">
         <v>876</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="I6" s="0" t="s">
+        <v>876</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="str">
+        <f aca="false">CONCATENATE("celexd:",B7)</f>
+        <v>celexd:5_IE</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>877</v>
       </c>
-      <c r="I6" s="0" t="s">
-        <v>877</v>
-      </c>
-      <c r="J6" s="0" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="C7" s="0" t="s">
         <v>878</v>
       </c>
-      <c r="B7" s="0" t="s">
-        <v>703</v>
-      </c>
-      <c r="C7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>879</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>880</v>
-      </c>
       <c r="E7" s="0" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G7" s="0" t="s">
+        <v>880</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>876</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>876</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="str">
+        <f aca="false">CONCATENATE("celexd:",B8)</f>
+        <v>celexd:5_AG</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>881</v>
       </c>
-      <c r="H7" s="0" t="s">
-        <v>877</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>877</v>
-      </c>
-      <c r="J7" s="0" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="C8" s="0" t="s">
         <v>882</v>
       </c>
-      <c r="B8" s="0" t="s">
-        <v>718</v>
-      </c>
-      <c r="C8" s="0" t="s">
+      <c r="D8" s="2" t="s">
         <v>883</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="0" t="s">
         <v>884</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>885</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G8" s="0" t="s">
+        <v>885</v>
+      </c>
+      <c r="H8" s="0" t="s">
         <v>886</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="I8" s="0" t="s">
         <v>887</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="J8" s="0" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="str">
+        <f aca="false">CONCATENATE("celexd:",B9)</f>
+        <v>celexd:5_PC_EUR</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>888</v>
       </c>
-      <c r="J8" s="0" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="C9" s="0" t="s">
         <v>889</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>729</v>
-      </c>
-      <c r="C9" s="0" t="s">
+      <c r="D9" s="2" t="s">
         <v>890</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="0" t="s">
         <v>891</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>892</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G9" s="0" t="s">
+        <v>892</v>
+      </c>
+      <c r="H9" s="0" t="s">
         <v>893</v>
       </c>
-      <c r="H9" s="0" t="s">
+      <c r="I9" s="0" t="s">
+        <v>893</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="str">
+        <f aca="false">CONCATENATE("celexd:",B10)</f>
+        <v>celexd:6_CA</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>894</v>
       </c>
-      <c r="I9" s="0" t="s">
-        <v>894</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="C10" s="0" t="s">
         <v>895</v>
       </c>
-      <c r="B10" s="0" t="s">
-        <v>778</v>
-      </c>
-      <c r="C10" s="0" t="s">
+      <c r="D10" s="0" t="s">
         <v>896</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="E10" s="0" t="s">
         <v>897</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>898</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>6</v>
       </c>
       <c r="G10" s="0" t="s">
+        <v>898</v>
+      </c>
+      <c r="H10" s="0" t="s">
         <v>899</v>
       </c>
-      <c r="H10" s="0" t="s">
+      <c r="I10" s="0" t="s">
+        <v>899</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="str">
+        <f aca="false">CONCATENATE("celexd:",B11)</f>
+        <v>celexd:6_CB</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>900</v>
       </c>
-      <c r="I10" s="0" t="s">
-        <v>900</v>
-      </c>
-      <c r="J10" s="0" t="s">
-        <v>859</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="C11" s="0" t="s">
         <v>901</v>
       </c>
-      <c r="B11" s="0" t="s">
-        <v>787</v>
-      </c>
-      <c r="C11" s="0" t="s">
+      <c r="D11" s="0" t="s">
         <v>902</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>903</v>
-      </c>
       <c r="E11" s="0" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>6</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
     </row>
   </sheetData>
@@ -14702,7 +14709,7 @@
   <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14712,247 +14719,247 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>904</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>905</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>906</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>907</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>908</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>909</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>909</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>910</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>911</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>911</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>912</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>913</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>913</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>914</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>915</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>915</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>916</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>917</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>917</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>918</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>919</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>919</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>920</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>921</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>921</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>922</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>923</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>923</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>924</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>925</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>925</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>926</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>927</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>927</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>928</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>929</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>929</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>930</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>931</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>931</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>932</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>933</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>933</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>934</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>935</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
+        <v>935</v>
+      </c>
+      <c r="B17" s="0" t="s">
         <v>936</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>937</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>937</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>938</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>939</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
+        <v>939</v>
+      </c>
+      <c r="B19" s="0" t="s">
         <v>940</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>941</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>941</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>942</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>943</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>943</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>944</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>945</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>945</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>946</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>947</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>947</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>948</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>949</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>949</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>950</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>951</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>951</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>952</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>953</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>954</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>955</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>956</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>958</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>959</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>960</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>960</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>961</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>962</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
* create final draft of the LAM-SKOS-AP source * need to add collection statements * need to validate with SHACL constraint checker
</commit_message>
<xml_diff>
--- a/docs/semi-structured/LAM_metadata_03.xlsx
+++ b/docs/semi-structured/LAM_metadata_03.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="LAM metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3533" uniqueCount="962">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3539" uniqueCount="969">
   <si>
     <t xml:space="preserve">URI</t>
   </si>
@@ -2345,10 +2345,10 @@
     <t xml:space="preserve">cdm:act_preparatory</t>
   </si>
   <si>
-    <t xml:space="preserve">COM | and Service/DG responsible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">REG_DRAFT</t>
+    <t xml:space="preserve">cobo:COM | and Service/DG responsible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rety:REG_DRAFT</t>
   </si>
   <si>
     <t xml:space="preserve">YU</t>
@@ -2407,7 +2407,26 @@
     <t xml:space="preserve">31998Y0307(02)</t>
   </si>
   <si>
-    <t xml:space="preserve">DIR_DRAFT</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">cobo:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">COM | and Service/DG responsible</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">rety:DIR_DRAFT</t>
   </si>
   <si>
     <t xml:space="preserve">lamd:c_003</t>
@@ -2431,7 +2450,7 @@
 31997Y1203(01)</t>
   </si>
   <si>
-    <t xml:space="preserve">COMMUNIC_DRAFT</t>
+    <t xml:space="preserve">rety:COMMUNIC_DRAFT</t>
   </si>
   <si>
     <t xml:space="preserve">fd:fd_365/DATPUB</t>
@@ -2457,7 +2476,7 @@
     <t xml:space="preserve">JOC_1990_044_R_0014_01</t>
   </si>
   <si>
-    <t xml:space="preserve">DECLAR_DRAFT</t>
+    <t xml:space="preserve">rety:DECLAR_DRAFT</t>
   </si>
   <si>
     <t xml:space="preserve">lamd:c_005</t>
@@ -2480,10 +2499,26 @@
     <t xml:space="preserve">cdm:opinion_other_committee_ecsc</t>
   </si>
   <si>
-    <t xml:space="preserve">EESC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">OPIN_EXPLOR</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">cobo:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">EESC</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">rety:OPIN_EXPLOR</t>
   </si>
   <si>
     <t xml:space="preserve">celexd:5_AE</t>
@@ -2544,7 +2579,7 @@
     <t xml:space="preserve">cdm:opinion_consultation_eesc</t>
   </si>
   <si>
-    <t xml:space="preserve">OPIN</t>
+    <t xml:space="preserve">rety:OPIN</t>
   </si>
   <si>
     <t xml:space="preserve">Y| Link to proposal (COM document)</t>
@@ -2593,7 +2628,7 @@
 52014IE1468</t>
   </si>
   <si>
-    <t xml:space="preserve">OWNINI_OPIN</t>
+    <t xml:space="preserve">rety:OWNINI_OPIN</t>
   </si>
   <si>
     <t xml:space="preserve">celexd:5_IE</t>
@@ -2616,7 +2651,7 @@
 52012IE2321</t>
   </si>
   <si>
-    <t xml:space="preserve">OWNINI_OPIN_ADDIT</t>
+    <t xml:space="preserve">rety:OWNINI_OPIN_ADDIT</t>
   </si>
   <si>
     <t xml:space="preserve">lamd:c_010</t>
@@ -2640,10 +2675,10 @@
     <t xml:space="preserve">cdm:position_council</t>
   </si>
   <si>
-    <t xml:space="preserve">CONSIL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">STAT_REASON</t>
+    <t xml:space="preserve">cobo:CONSIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rety:STAT_REASON</t>
   </si>
   <si>
     <t xml:space="preserve">celexd:5_AG</t>
@@ -2681,7 +2716,7 @@
     <t xml:space="preserve">cdm:proposal_regulation_ec</t>
   </si>
   <si>
-    <t xml:space="preserve">PROP_REG</t>
+    <t xml:space="preserve">rety:PROP_REG</t>
   </si>
   <si>
     <t xml:space="preserve">celexd:5_PC_EUR</t>
@@ -2754,7 +2789,7 @@
     <t xml:space="preserve">52015PC0049</t>
   </si>
   <si>
-    <t xml:space="preserve">AMEND_PROP_REG</t>
+    <t xml:space="preserve">rety:AMEND_PROP_REG</t>
   </si>
   <si>
     <t xml:space="preserve">lamd:c_014</t>
@@ -2782,7 +2817,7 @@
     <t xml:space="preserve">cdm:proposal_directive_ec</t>
   </si>
   <si>
-    <t xml:space="preserve">PROP_DIR</t>
+    <t xml:space="preserve">rety:PROP_DIR</t>
   </si>
   <si>
     <t xml:space="preserve">lamd:c_015</t>
@@ -2835,7 +2870,7 @@
     <t xml:space="preserve">52017PC0637</t>
   </si>
   <si>
-    <t xml:space="preserve">AMEND_PROP_DIR</t>
+    <t xml:space="preserve">rety:AMEND_PROP_DIR</t>
   </si>
   <si>
     <t xml:space="preserve">lamd:c_017</t>
@@ -2861,10 +2896,10 @@
     <t xml:space="preserve">cdm:info_decision_cjeu</t>
   </si>
   <si>
-    <t xml:space="preserve">CJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">INFO_JUDICIAL</t>
+    <t xml:space="preserve">cobo:CJ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rety:INFO_JUDICIAL</t>
   </si>
   <si>
     <t xml:space="preserve">celexd:6_CA</t>
@@ -2920,10 +2955,10 @@
     <t xml:space="preserve">cdm:resource_legal</t>
   </si>
   <si>
-    <t xml:space="preserve">EURUN | and country</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ARRANG</t>
+    <t xml:space="preserve">cobo:EURUN | and country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rety:ARRANG</t>
   </si>
   <si>
     <t xml:space="preserve">celexd:2_A_OJL</t>
@@ -2957,13 +2992,13 @@
     <t xml:space="preserve">52016XC0430(01)</t>
   </si>
   <si>
-    <t xml:space="preserve">COM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NOTICE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">eurovoc.europa.eu/2809</t>
+    <t xml:space="preserve">cobo:COM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rety:NOTICE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eurovoc:2809</t>
   </si>
   <si>
     <t xml:space="preserve">at:subject-matter/DGEN</t>
@@ -3452,6 +3487,24 @@
   <si>
     <t xml:space="preserve">http://www.w3.org/ns/shacl#</t>
   </si>
+  <si>
+    <t xml:space="preserve">cobo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://publications.europa.eu/resource/authority/corporate-body/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rety</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://publications.europa.eu/resource/authority/resource-type/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">eurovoc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://eurovoc.europa.eu/</t>
+  </si>
 </sst>
 </file>
 
@@ -3460,7 +3513,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3488,6 +3541,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -3565,7 +3623,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3586,6 +3644,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3596,6 +3658,10 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -3680,9 +3746,9 @@
   <dimension ref="A1:AB107"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B93" activeCellId="0" sqref="B93"/>
+      <selection pane="bottomLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7838,10 +7904,10 @@
   </sheetPr>
   <dimension ref="A1:CR21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="K23" activeCellId="0" sqref="K23"/>
+      <selection pane="bottomLeft" activeCell="M21" activeCellId="0" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7854,7 +7920,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="22.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="31.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="29.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="18.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="21.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="3.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="16.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="9.16"/>
@@ -8523,7 +8589,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="41.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
         <v>646</v>
       </c>
@@ -8545,11 +8611,11 @@
       <c r="G3" s="3" t="s">
         <v>630</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>631</v>
+      <c r="H3" s="5" t="s">
+        <v>651</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>633</v>
@@ -8813,33 +8879,33 @@
         <v>645</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="41.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>630</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>631</v>
+      <c r="H4" s="5" t="s">
+        <v>651</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>633</v>
@@ -8866,7 +8932,7 @@
         <v>636</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="S4" s="3" t="s">
         <v>635</v>
@@ -9103,33 +9169,33 @@
         <v>645</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="41.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>630</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>631</v>
+      <c r="H5" s="5" t="s">
+        <v>651</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="J5" s="3" t="s">
         <v>633</v>
@@ -9156,7 +9222,7 @@
         <v>636</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="S5" s="3" t="s">
         <v>635</v>
@@ -9393,36 +9459,36 @@
         <v>645</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="27.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>668</v>
-      </c>
-      <c r="C6" s="5" t="s">
         <v>669</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="C6" s="6" t="s">
         <v>670</v>
       </c>
+      <c r="D6" s="6" t="s">
+        <v>671</v>
+      </c>
       <c r="F6" s="4" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>672</v>
-      </c>
-      <c r="H6" s="3" t="s">
         <v>673</v>
       </c>
+      <c r="H6" s="5" t="s">
+        <v>674</v>
+      </c>
       <c r="I6" s="3" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>633</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>635</v>
@@ -9443,7 +9509,7 @@
         <v>636</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="S6" s="3" t="s">
         <v>635</v>
@@ -9506,7 +9572,7 @@
         <v>635</v>
       </c>
       <c r="AM6" s="3" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="AN6" s="3" t="s">
         <v>635</v>
@@ -9533,7 +9599,7 @@
         <v>636</v>
       </c>
       <c r="AV6" s="3" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="AW6" s="3" t="s">
         <v>635</v>
@@ -9674,45 +9740,45 @@
         <v>643</v>
       </c>
       <c r="CQ6" s="3" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="CR6" s="3" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="229.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="323.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>682</v>
-      </c>
-      <c r="C7" s="5" t="s">
         <v>683</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="C7" s="6" t="s">
         <v>684</v>
       </c>
+      <c r="D7" s="7" t="s">
+        <v>685</v>
+      </c>
       <c r="E7" s="4" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>673</v>
+        <v>688</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>674</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>633</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>635</v>
@@ -9733,7 +9799,7 @@
         <v>636</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="S7" s="3" t="s">
         <v>635</v>
@@ -9796,7 +9862,7 @@
         <v>635</v>
       </c>
       <c r="AM7" s="3" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="AN7" s="3" t="s">
         <v>635</v>
@@ -9907,10 +9973,10 @@
         <v>635</v>
       </c>
       <c r="BX7" s="3" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="BY7" s="3" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="BZ7" s="3" t="s">
         <v>641</v>
@@ -9922,7 +9988,7 @@
         <v>635</v>
       </c>
       <c r="CC7" s="3" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="CD7" s="3" t="s">
         <v>635</v>
@@ -9964,45 +10030,45 @@
         <v>643</v>
       </c>
       <c r="CQ7" s="3" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="CR7" s="3" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>692</v>
-      </c>
-      <c r="C8" s="5" t="s">
         <v>693</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="C8" s="6" t="s">
         <v>694</v>
       </c>
+      <c r="D8" s="6" t="s">
+        <v>695</v>
+      </c>
       <c r="E8" s="3" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>687</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>673</v>
+        <v>688</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>674</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>633</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="L8" s="3" t="s">
         <v>635</v>
@@ -10023,7 +10089,7 @@
         <v>636</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="S8" s="3" t="s">
         <v>635</v>
@@ -10086,7 +10152,7 @@
         <v>635</v>
       </c>
       <c r="AM8" s="3" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="AN8" s="3" t="s">
         <v>635</v>
@@ -10197,7 +10263,7 @@
         <v>635</v>
       </c>
       <c r="BX8" s="3" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="BY8" s="3" t="s">
         <v>635</v>
@@ -10212,7 +10278,7 @@
         <v>635</v>
       </c>
       <c r="CC8" s="3" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="CD8" s="3" t="s">
         <v>635</v>
@@ -10254,42 +10320,42 @@
         <v>643</v>
       </c>
       <c r="CQ8" s="3" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="CR8" s="3" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>698</v>
-      </c>
-      <c r="C9" s="5" t="s">
         <v>699</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="C9" s="6" t="s">
         <v>700</v>
       </c>
+      <c r="D9" s="6" t="s">
+        <v>701</v>
+      </c>
       <c r="F9" s="4" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>672</v>
-      </c>
-      <c r="H9" s="3" t="s">
         <v>673</v>
       </c>
+      <c r="H9" s="5" t="s">
+        <v>674</v>
+      </c>
       <c r="I9" s="3" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>633</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>635</v>
@@ -10310,7 +10376,7 @@
         <v>636</v>
       </c>
       <c r="R9" s="3" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="S9" s="3" t="s">
         <v>635</v>
@@ -10373,7 +10439,7 @@
         <v>635</v>
       </c>
       <c r="AM9" s="3" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="AN9" s="3" t="s">
         <v>635</v>
@@ -10400,7 +10466,7 @@
         <v>636</v>
       </c>
       <c r="AV9" s="3" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="AW9" s="3" t="s">
         <v>635</v>
@@ -10541,42 +10607,42 @@
         <v>643</v>
       </c>
       <c r="CQ9" s="3" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="CR9" s="3" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>705</v>
-      </c>
-      <c r="C10" s="5" t="s">
         <v>706</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="C10" s="6" t="s">
         <v>707</v>
       </c>
+      <c r="D10" s="6" t="s">
+        <v>708</v>
+      </c>
       <c r="F10" s="4" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>672</v>
-      </c>
-      <c r="H10" s="3" t="s">
         <v>673</v>
       </c>
+      <c r="H10" s="5" t="s">
+        <v>674</v>
+      </c>
       <c r="I10" s="3" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>633</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>635</v>
@@ -10597,7 +10663,7 @@
         <v>636</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="S10" s="3" t="s">
         <v>635</v>
@@ -10660,7 +10726,7 @@
         <v>635</v>
       </c>
       <c r="AM10" s="3" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="AN10" s="3" t="s">
         <v>635</v>
@@ -10687,7 +10753,7 @@
         <v>636</v>
       </c>
       <c r="AV10" s="3" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="AW10" s="3" t="s">
         <v>635</v>
@@ -10828,42 +10894,42 @@
         <v>643</v>
       </c>
       <c r="CQ10" s="3" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="CR10" s="3" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>711</v>
-      </c>
-      <c r="C11" s="5" t="s">
         <v>712</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="C11" s="6" t="s">
         <v>713</v>
       </c>
+      <c r="D11" s="6" t="s">
+        <v>714</v>
+      </c>
       <c r="F11" s="4" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>633</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>635</v>
@@ -10884,13 +10950,13 @@
         <v>636</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="S11" s="3" t="s">
         <v>635</v>
       </c>
       <c r="T11" s="3" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="U11" s="3" t="s">
         <v>635</v>
@@ -11058,7 +11124,7 @@
         <v>635</v>
       </c>
       <c r="BX11" s="3" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="BY11" s="3" t="s">
         <v>635</v>
@@ -11073,7 +11139,7 @@
         <v>635</v>
       </c>
       <c r="CC11" s="3" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="CD11" s="3" t="s">
         <v>635</v>
@@ -11115,42 +11181,42 @@
         <v>643</v>
       </c>
       <c r="CQ11" s="3" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>631</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>633</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="L12" s="3" t="s">
         <v>635</v>
@@ -11177,10 +11243,10 @@
         <v>635</v>
       </c>
       <c r="T12" s="4" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="U12" s="3" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="V12" s="3" t="s">
         <v>635</v>
@@ -11216,7 +11282,7 @@
         <v>635</v>
       </c>
       <c r="AG12" s="3" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="AH12" s="3" t="s">
         <v>641</v>
@@ -11348,7 +11414,7 @@
         <v>635</v>
       </c>
       <c r="BY12" s="3" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="BZ12" s="3" t="s">
         <v>641</v>
@@ -11360,7 +11426,7 @@
         <v>635</v>
       </c>
       <c r="CC12" s="3" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="CD12" s="3" t="s">
         <v>635</v>
@@ -11405,42 +11471,42 @@
         <v>644</v>
       </c>
       <c r="CR12" s="3" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="108.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>631</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>633</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>635</v>
@@ -11467,10 +11533,10 @@
         <v>635</v>
       </c>
       <c r="T13" s="4" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="U13" s="3" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="V13" s="3" t="s">
         <v>635</v>
@@ -11650,7 +11716,7 @@
         <v>635</v>
       </c>
       <c r="CC13" s="3" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="CD13" s="3" t="s">
         <v>635</v>
@@ -11695,42 +11761,42 @@
         <v>644</v>
       </c>
       <c r="CR13" s="3" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>741</v>
-      </c>
-      <c r="B14" s="7" t="s">
         <v>742</v>
       </c>
+      <c r="B14" s="8" t="s">
+        <v>743</v>
+      </c>
       <c r="C14" s="4" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>631</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>633</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="L14" s="3" t="s">
         <v>635</v>
@@ -11757,10 +11823,10 @@
         <v>635</v>
       </c>
       <c r="T14" s="4" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="U14" s="3" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="V14" s="3" t="s">
         <v>635</v>
@@ -11940,7 +12006,7 @@
         <v>635</v>
       </c>
       <c r="CC14" s="3" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="CD14" s="3" t="s">
         <v>635</v>
@@ -11985,42 +12051,42 @@
         <v>644</v>
       </c>
       <c r="CR14" s="3" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>631</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="J15" s="3" t="s">
         <v>633</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="L15" s="3" t="s">
         <v>635</v>
@@ -12047,10 +12113,10 @@
         <v>635</v>
       </c>
       <c r="T15" s="4" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="U15" s="3" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="V15" s="3" t="s">
         <v>635</v>
@@ -12086,7 +12152,7 @@
         <v>635</v>
       </c>
       <c r="AG15" s="3" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="AH15" s="3" t="s">
         <v>641</v>
@@ -12218,7 +12284,7 @@
         <v>635</v>
       </c>
       <c r="BY15" s="3" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="BZ15" s="3" t="s">
         <v>641</v>
@@ -12230,7 +12296,7 @@
         <v>635</v>
       </c>
       <c r="CC15" s="3" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="CD15" s="3" t="s">
         <v>635</v>
@@ -12275,42 +12341,42 @@
         <v>644</v>
       </c>
       <c r="CR15" s="3" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>631</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>633</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="L16" s="3" t="s">
         <v>635</v>
@@ -12337,10 +12403,10 @@
         <v>635</v>
       </c>
       <c r="T16" s="4" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="U16" s="3" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="V16" s="3" t="s">
         <v>635</v>
@@ -12520,7 +12586,7 @@
         <v>635</v>
       </c>
       <c r="CC16" s="3" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="CD16" s="3" t="s">
         <v>635</v>
@@ -12565,42 +12631,42 @@
         <v>644</v>
       </c>
       <c r="CR16" s="3" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>762</v>
-      </c>
-      <c r="B17" s="7" t="s">
         <v>763</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="B17" s="8" t="s">
         <v>764</v>
       </c>
+      <c r="C17" s="8" t="s">
+        <v>765</v>
+      </c>
       <c r="D17" s="4" t="s">
-        <v>765</v>
-      </c>
-      <c r="E17" s="7" t="s">
         <v>766</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="E17" s="8" t="s">
         <v>767</v>
       </c>
+      <c r="F17" s="8" t="s">
+        <v>768</v>
+      </c>
       <c r="G17" s="3" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>631</v>
       </c>
-      <c r="I17" s="7" t="s">
-        <v>768</v>
+      <c r="I17" s="8" t="s">
+        <v>769</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>633</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>635</v>
@@ -12627,10 +12693,10 @@
         <v>635</v>
       </c>
       <c r="T17" s="4" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="U17" s="3" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="V17" s="3" t="s">
         <v>635</v>
@@ -12810,7 +12876,7 @@
         <v>635</v>
       </c>
       <c r="CC17" s="3" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="CD17" s="3" t="s">
         <v>635</v>
@@ -12855,48 +12921,48 @@
         <v>644</v>
       </c>
       <c r="CR17" s="3" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>633</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>635</v>
       </c>
       <c r="M18" s="3" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="N18" s="3" t="s">
         <v>635</v>
@@ -13133,57 +13199,57 @@
         <v>635</v>
       </c>
       <c r="CN18" s="3" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="CO18" s="3" t="s">
         <v>635</v>
       </c>
       <c r="CP18" s="3" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="CQ18" s="3" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="J19" s="3" t="s">
         <v>633</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="L19" s="3" t="s">
         <v>635</v>
       </c>
       <c r="M19" s="3" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="N19" s="3" t="s">
         <v>635</v>
@@ -13420,48 +13486,48 @@
         <v>635</v>
       </c>
       <c r="CN19" s="3" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="CO19" s="3" t="s">
         <v>635</v>
       </c>
       <c r="CP19" s="3" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="CQ19" s="3" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="J20" s="3" t="s">
         <v>633</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="L20" s="3" t="s">
         <v>635</v>
@@ -13482,7 +13548,7 @@
         <v>636</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="S20" s="3" t="s">
         <v>636</v>
@@ -13503,7 +13569,7 @@
         <v>636</v>
       </c>
       <c r="Y20" s="3" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="Z20" s="3" t="s">
         <v>635</v>
@@ -13710,36 +13776,36 @@
         <v>635</v>
       </c>
       <c r="CP20" s="3" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="CQ20" s="3" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>630</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>633</v>
@@ -13751,13 +13817,13 @@
         <v>635</v>
       </c>
       <c r="M21" s="3" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="N21" s="3" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="P21" s="3" t="s">
         <v>635</v>
@@ -13766,7 +13832,7 @@
         <v>636</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="S21" s="3" t="s">
         <v>635</v>
@@ -13892,7 +13958,7 @@
         <v>635</v>
       </c>
       <c r="BH21" s="3" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="BI21" s="3" t="s">
         <v>635</v>
@@ -13955,7 +14021,7 @@
         <v>635</v>
       </c>
       <c r="CC21" s="3" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="CD21" s="3" t="s">
         <v>635</v>
@@ -14000,7 +14066,7 @@
         <v>644</v>
       </c>
       <c r="CR21" s="3" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
     </row>
   </sheetData>
@@ -14021,8 +14087,8 @@
   </sheetPr>
   <dimension ref="A1:AB8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AA1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AB2" activeCellId="0" sqref="AB2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="X1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X1" activeCellId="0" sqref="X1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14055,7 +14121,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>7</v>
@@ -14123,25 +14189,25 @@
     </row>
     <row r="2" customFormat="false" ht="176.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="Z2" s="0" t="s">
         <v>72</v>
@@ -14155,22 +14221,22 @@
     </row>
     <row r="3" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="Z3" s="0" t="s">
         <v>72</v>
@@ -14184,25 +14250,25 @@
     </row>
     <row r="4" customFormat="false" ht="149.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="U4" s="0" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="Z4" s="0" t="s">
         <v>72</v>
@@ -14216,25 +14282,25 @@
     </row>
     <row r="5" customFormat="false" ht="95.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="T5" s="2" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="U5" s="0" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="Z5" s="0" t="s">
         <v>72</v>
@@ -14248,7 +14314,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>29</v>
@@ -14262,7 +14328,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>33</v>
@@ -14271,33 +14337,33 @@
         <v>34</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="82.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="U8" s="0" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="Z8" s="0" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="AA8" s="0" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
     </row>
   </sheetData>
@@ -14354,19 +14420,19 @@
         <v>50</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14375,28 +14441,28 @@
         <v>celexd:2_A_OJL</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>2</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14405,31 +14471,31 @@
         <v>celexd:2_A_OJC</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14438,28 +14504,28 @@
         <v>celexd:5_XC_OJL</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14468,28 +14534,28 @@
         <v>celexd:5_XC_OJC</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14498,31 +14564,31 @@
         <v>celexd:5_AE</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14531,31 +14597,31 @@
         <v>celexd:5_IE</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14564,31 +14630,31 @@
         <v>celexd:5_AG</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14597,31 +14663,31 @@
         <v>celexd:5_PC_EUR</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14630,31 +14696,31 @@
         <v>celexd:6_CA</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>6</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14663,31 +14729,31 @@
         <v>celexd:6_CB</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>6</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
     </row>
   </sheetData>
@@ -14708,8 +14774,8 @@
   </sheetPr>
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14719,253 +14785,278 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="1" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>961</v>
-      </c>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>962</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>963</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>964</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="s">
+        <v>965</v>
+      </c>
+      <c r="B33" s="9" t="s">
+        <v>966</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="s">
+        <v>967</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>968</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B32" r:id="rId1" display="http://publications.europa.eu/resource/authority/corporate-body/"/>
+    <hyperlink ref="B33" r:id="rId2" display="http://publications.europa.eu/resource/authority/resource-type/"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
* add /deliverable folder * start writing the requirements analise using DITA
</commit_message>
<xml_diff>
--- a/docs/semi-structured/LAM_metadata_03.xlsx
+++ b/docs/semi-structured/LAM_metadata_03.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LAM metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3734" uniqueCount="1008">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3734" uniqueCount="1009">
   <si>
     <t xml:space="preserve">URI</t>
   </si>
@@ -199,7 +199,7 @@
     <t xml:space="preserve">Label of the concept</t>
   </si>
   <si>
-    <t xml:space="preserve">skosxl:prefLabel@en</t>
+    <t xml:space="preserve">skos:prefLabel@en</t>
   </si>
   <si>
     <t xml:space="preserve">KEYWORD</t>
@@ -3312,6 +3312,9 @@
   </si>
   <si>
     <t xml:space="preserve">lamd:md_CODE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">skosxl:prefLabel@en</t>
   </si>
   <si>
     <t xml:space="preserve">lamd:md_LABEL</t>
@@ -3895,10 +3898,10 @@
   </sheetPr>
   <dimension ref="A1:AI1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B108" activeCellId="0" sqref="B108"/>
+      <selection pane="bottomLeft" activeCell="D110" activeCellId="0" sqref="D110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11297,7 +11300,7 @@
   </sheetPr>
   <dimension ref="A1:CR21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
@@ -17480,7 +17483,7 @@
   </sheetPr>
   <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -17790,8 +17793,8 @@
   </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18180,8 +18183,8 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G35" activeCellId="0" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18622,7 +18625,7 @@
   </sheetPr>
   <dimension ref="A1:B112"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -18651,18 +18654,18 @@
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>40</v>
+        <v>898</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>40</v>
+        <v>898</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18670,7 +18673,7 @@
         <v>46</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18678,7 +18681,7 @@
         <v>50</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18686,7 +18689,7 @@
         <v>53</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18694,7 +18697,7 @@
         <v>57</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18702,7 +18705,7 @@
         <v>60</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18710,7 +18713,7 @@
         <v>64</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18718,7 +18721,7 @@
         <v>74</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18726,7 +18729,7 @@
         <v>82</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18734,7 +18737,7 @@
         <v>90</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18742,7 +18745,7 @@
         <v>93</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18750,7 +18753,7 @@
         <v>99</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18758,7 +18761,7 @@
         <v>104</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18766,7 +18769,7 @@
         <v>108</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18774,7 +18777,7 @@
         <v>112</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18782,7 +18785,7 @@
         <v>116</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18790,7 +18793,7 @@
         <v>126</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18798,7 +18801,7 @@
         <v>134</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18806,7 +18809,7 @@
         <v>143</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18814,7 +18817,7 @@
         <v>150</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18822,7 +18825,7 @@
         <v>157</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18830,7 +18833,7 @@
         <v>164</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18838,7 +18841,7 @@
         <v>171</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18846,7 +18849,7 @@
         <v>178</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18854,7 +18857,7 @@
         <v>184</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18862,7 +18865,7 @@
         <v>191</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18870,7 +18873,7 @@
         <v>197</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18878,7 +18881,7 @@
         <v>204</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18886,7 +18889,7 @@
         <v>207</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18894,7 +18897,7 @@
         <v>210</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18902,7 +18905,7 @@
         <v>214</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18910,7 +18913,7 @@
         <v>217</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18918,7 +18921,7 @@
         <v>220</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18926,7 +18929,7 @@
         <v>224</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18934,7 +18937,7 @@
         <v>227</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18942,7 +18945,7 @@
         <v>230</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18950,7 +18953,7 @@
         <v>234</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18958,7 +18961,7 @@
         <v>238</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18966,7 +18969,7 @@
         <v>242</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18974,7 +18977,7 @@
         <v>246</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18982,7 +18985,7 @@
         <v>250</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18990,7 +18993,7 @@
         <v>253</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18998,7 +19001,7 @@
         <v>257</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19006,7 +19009,7 @@
         <v>261</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19014,7 +19017,7 @@
         <v>271</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19022,7 +19025,7 @@
         <v>286</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19030,7 +19033,7 @@
         <v>290</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19038,7 +19041,7 @@
         <v>294</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19046,7 +19049,7 @@
         <v>298</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19054,7 +19057,7 @@
         <v>304</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19062,7 +19065,7 @@
         <v>308</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19070,7 +19073,7 @@
         <v>312</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19078,7 +19081,7 @@
         <v>317</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19086,7 +19089,7 @@
         <v>321</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19094,7 +19097,7 @@
         <v>325</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19102,7 +19105,7 @@
         <v>329</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19110,7 +19113,7 @@
         <v>333</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19118,7 +19121,7 @@
         <v>338</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19126,7 +19129,7 @@
         <v>342</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19134,7 +19137,7 @@
         <v>346</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19142,7 +19145,7 @@
         <v>350</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19150,7 +19153,7 @@
         <v>354</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19158,7 +19161,7 @@
         <v>358</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19166,7 +19169,7 @@
         <v>362</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19174,7 +19177,7 @@
         <v>366</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19182,7 +19185,7 @@
         <v>370</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19190,7 +19193,7 @@
         <v>374</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19198,7 +19201,7 @@
         <v>377</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19206,7 +19209,7 @@
         <v>380</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19214,7 +19217,7 @@
         <v>384</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19222,7 +19225,7 @@
         <v>387</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19230,7 +19233,7 @@
         <v>390</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19238,7 +19241,7 @@
         <v>395</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19246,7 +19249,7 @@
         <v>398</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19254,7 +19257,7 @@
         <v>404</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19262,7 +19265,7 @@
         <v>409</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19270,7 +19273,7 @@
         <v>412</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19278,7 +19281,7 @@
         <v>417</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19286,7 +19289,7 @@
         <v>422</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19294,7 +19297,7 @@
         <v>425</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19302,7 +19305,7 @@
         <v>429</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19310,7 +19313,7 @@
         <v>433</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19318,7 +19321,7 @@
         <v>437</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19326,7 +19329,7 @@
         <v>440</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19334,7 +19337,7 @@
         <v>443</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19342,7 +19345,7 @@
         <v>446</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19350,7 +19353,7 @@
         <v>449</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19358,7 +19361,7 @@
         <v>452</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19366,7 +19369,7 @@
         <v>455</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19374,7 +19377,7 @@
         <v>117</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19382,7 +19385,7 @@
         <v>127</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19390,7 +19393,7 @@
         <v>262</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19398,7 +19401,7 @@
         <v>264</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19406,7 +19409,7 @@
         <v>265</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19414,7 +19417,7 @@
         <v>266</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19422,7 +19425,7 @@
         <v>272</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19430,7 +19433,7 @@
         <v>273</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19438,7 +19441,7 @@
         <v>275</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19446,7 +19449,7 @@
         <v>277</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19454,7 +19457,7 @@
         <v>278</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19462,7 +19465,7 @@
         <v>279</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19470,7 +19473,7 @@
         <v>280</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>1000</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19478,7 +19481,7 @@
         <v>399</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>1001</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19486,7 +19489,7 @@
         <v>400</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>1002</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19494,7 +19497,7 @@
         <v>523</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>1003</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19502,7 +19505,7 @@
         <v>529</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>1004</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19510,7 +19513,7 @@
         <v>534</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>1005</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19518,7 +19521,7 @@
         <v>540</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>1006</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19526,7 +19529,7 @@
         <v>546</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>1007</v>
+        <v>1008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add v4 of the input data with cleaned up "empty" rows
</commit_message>
<xml_diff>
--- a/docs/semi-structured/LAM_metadata_03.xlsx
+++ b/docs/semi-structured/LAM_metadata_03.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="LAM metadata" sheetId="1" state="visible" r:id="rId2"/>
@@ -72,12 +72,27 @@
         </r>
       </text>
     </comment>
+    <comment ref="J1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">This column replaces the propoerty with the LAM:propoerty URI extracted in a separate worksheet for convenience purpose only. Ideally the references hould be primarely done to these uris and no mapping should be used.
+ </t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3734" uniqueCount="1009">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3742" uniqueCount="1008">
   <si>
     <t xml:space="preserve">URI</t>
   </si>
@@ -2854,9 +2869,6 @@
   </si>
   <si>
     <t xml:space="preserve">Withdrawals</t>
-  </si>
-  <si>
-    <t xml:space="preserve">controlled value_annotation_1 </t>
   </si>
   <si>
     <t xml:space="preserve">skosxl:prefLabel</t>
@@ -3768,7 +3780,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3803,10 +3815,6 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -3898,10 +3906,10 @@
   </sheetPr>
   <dimension ref="A1:AI1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D110" activeCellId="0" sqref="D110"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="T1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="T1" activeCellId="0" sqref="T1"/>
+      <selection pane="bottomLeft" activeCell="E1" activeCellId="0" sqref="E1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3913,25 +3921,25 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="38.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="20.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="22.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="11.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="32.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="17.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="11.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="11.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="22.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="13.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="11.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="11.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="22.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="16.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="11.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="11.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="22.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="18.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="11.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="11.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="103"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="53.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="110.11"/>
@@ -11300,10 +11308,10 @@
   </sheetPr>
   <dimension ref="A1:CR21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="N2" activeCellId="0" sqref="N2"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="N2" activeCellId="1" sqref="E1:Z1 N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11361,7 +11369,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="52" min="52" style="4" width="11.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="53" min="53" style="4" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="54" min="54" style="4" width="13.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="4" width="17.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="55" min="55" style="4" width="17.04"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="56" min="56" style="4" width="11.96"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="57" min="57" style="4" width="12.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="58" min="58" style="4" width="13.22"/>
@@ -17483,8 +17491,8 @@
   </sheetPr>
   <dimension ref="A1:AI8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1:Z1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17497,98 +17505,114 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="35" style="0" width="15.44"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="9" t="s">
+    <row r="1" s="2" customFormat="true" ht="42.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9" t="s">
-        <v>746</v>
-      </c>
-      <c r="I1" s="9" t="s">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9" t="s">
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9" t="s">
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9" t="s">
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9" t="s">
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="9" t="s">
+      <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9" t="s">
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="9" t="s">
+      <c r="X1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9" t="s">
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="9" t="s">
+      <c r="AA1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="9" t="s">
+      <c r="AB1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="9" t="s">
+      <c r="AC1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="9" t="s">
+      <c r="AD1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="9" t="s">
+      <c r="AE1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="9" t="s">
+      <c r="AF1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="9" t="s">
+      <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="9" t="s">
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="9" t="s">
+      <c r="AI1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="176.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="str">
         <f aca="false">CONCATENATE("celexd:md_",B2)</f>
         <v>celexd:md_DTS</v>
@@ -17744,7 +17768,7 @@
         <v>39</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17793,8 +17817,8 @@
   </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H12" activeCellId="0" sqref="H12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H12" activeCellId="1" sqref="E1:Z1 H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17841,7 +17865,7 @@
         <v>538</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17850,28 +17874,28 @@
         <v>celexd:c_2_A_OJL</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>748</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>749</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>750</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>751</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>2</v>
       </c>
       <c r="G2" s="0" t="s">
+        <v>751</v>
+      </c>
+      <c r="H2" s="0" t="s">
         <v>752</v>
       </c>
-      <c r="H2" s="0" t="s">
+      <c r="I2" s="0" t="s">
+        <v>752</v>
+      </c>
+      <c r="J2" s="0" t="s">
         <v>753</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>753</v>
-      </c>
-      <c r="J2" s="0" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17880,31 +17904,31 @@
         <v>celexd:c_2_A_OJC</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>754</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>749</v>
+      </c>
+      <c r="D3" s="0" t="s">
         <v>755</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>750</v>
-      </c>
-      <c r="D3" s="0" t="s">
+      <c r="E3" s="0" t="s">
         <v>756</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>757</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>2</v>
       </c>
       <c r="G3" s="0" t="s">
+        <v>751</v>
+      </c>
+      <c r="H3" s="0" t="s">
         <v>752</v>
       </c>
-      <c r="H3" s="0" t="s">
+      <c r="I3" s="0" t="s">
+        <v>752</v>
+      </c>
+      <c r="J3" s="0" t="s">
         <v>753</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>753</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17913,28 +17937,28 @@
         <v>celexd:c_5_XC_OJL</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>757</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>758</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>759</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>760</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="H4" s="0" t="s">
+        <v>752</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>752</v>
+      </c>
+      <c r="J4" s="0" t="s">
         <v>753</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>753</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17943,28 +17967,28 @@
         <v>celexd:c_5_XC_OJC</v>
       </c>
       <c r="B5" s="0" t="s">
+        <v>761</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>762</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>763</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>764</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="H5" s="0" t="s">
+        <v>752</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>752</v>
+      </c>
+      <c r="J5" s="0" t="s">
         <v>753</v>
-      </c>
-      <c r="I5" s="0" t="s">
-        <v>753</v>
-      </c>
-      <c r="J5" s="0" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17973,31 +17997,31 @@
         <v>celexd:c_5_AE</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>764</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>765</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>766</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="E6" s="0" t="s">
         <v>767</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>768</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G6" s="0" t="s">
+        <v>768</v>
+      </c>
+      <c r="H6" s="0" t="s">
         <v>769</v>
       </c>
-      <c r="H6" s="0" t="s">
-        <v>770</v>
-      </c>
       <c r="I6" s="0" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18006,31 +18030,31 @@
         <v>celexd:c_5_IE</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>770</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>771</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>772</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>773</v>
-      </c>
       <c r="E7" s="0" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18039,31 +18063,31 @@
         <v>celexd:c_5_AG</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>774</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>775</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>776</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="0" t="s">
         <v>777</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>778</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G8" s="0" t="s">
+        <v>778</v>
+      </c>
+      <c r="H8" s="0" t="s">
         <v>779</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="I8" s="0" t="s">
         <v>780</v>
       </c>
-      <c r="I8" s="0" t="s">
-        <v>781</v>
-      </c>
       <c r="J8" s="0" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18072,31 +18096,31 @@
         <v>celexd:c_5_PC_EUR</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>781</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>782</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>783</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="0" t="s">
         <v>784</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>785</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>5</v>
       </c>
       <c r="G9" s="0" t="s">
+        <v>785</v>
+      </c>
+      <c r="H9" s="0" t="s">
         <v>786</v>
       </c>
-      <c r="H9" s="0" t="s">
-        <v>787</v>
-      </c>
       <c r="I9" s="0" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18105,31 +18129,31 @@
         <v>celexd:c_6_CA</v>
       </c>
       <c r="B10" s="0" t="s">
+        <v>787</v>
+      </c>
+      <c r="C10" s="0" t="s">
         <v>788</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="D10" s="0" t="s">
         <v>789</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="E10" s="0" t="s">
         <v>790</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>791</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>6</v>
       </c>
       <c r="G10" s="0" t="s">
+        <v>791</v>
+      </c>
+      <c r="H10" s="0" t="s">
         <v>792</v>
       </c>
-      <c r="H10" s="0" t="s">
-        <v>793</v>
-      </c>
       <c r="I10" s="0" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18138,31 +18162,31 @@
         <v>celexd:c_6_CB</v>
       </c>
       <c r="B11" s="0" t="s">
+        <v>793</v>
+      </c>
+      <c r="C11" s="0" t="s">
         <v>794</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="D11" s="0" t="s">
         <v>795</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>796</v>
-      </c>
       <c r="E11" s="0" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>6</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
     </row>
   </sheetData>
@@ -18183,8 +18207,8 @@
   </sheetPr>
   <dimension ref="A1:B1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G35" activeCellId="0" sqref="G35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G35" activeCellId="1" sqref="E1:Z1 G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18195,415 +18219,415 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
+        <v>797</v>
+      </c>
+      <c r="B1" s="0" t="s">
         <v>798</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>799</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>800</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>801</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>802</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>802</v>
+      </c>
+      <c r="B4" s="0" t="s">
         <v>803</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>804</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
+        <v>804</v>
+      </c>
+      <c r="B5" s="0" t="s">
         <v>805</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>806</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
+        <v>806</v>
+      </c>
+      <c r="B6" s="0" t="s">
         <v>807</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>808</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
+        <v>808</v>
+      </c>
+      <c r="B7" s="0" t="s">
         <v>809</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>810</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>810</v>
+      </c>
+      <c r="B8" s="0" t="s">
         <v>811</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>812</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>812</v>
+      </c>
+      <c r="B9" s="0" t="s">
         <v>813</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>814</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
+        <v>814</v>
+      </c>
+      <c r="B10" s="0" t="s">
         <v>815</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>816</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
+        <v>816</v>
+      </c>
+      <c r="B11" s="0" t="s">
         <v>817</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>818</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
+        <v>818</v>
+      </c>
+      <c r="B12" s="0" t="s">
         <v>819</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>820</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
+        <v>820</v>
+      </c>
+      <c r="B13" s="0" t="s">
         <v>821</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>822</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
+        <v>822</v>
+      </c>
+      <c r="B14" s="0" t="s">
         <v>823</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>824</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
+        <v>824</v>
+      </c>
+      <c r="B15" s="0" t="s">
         <v>825</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
+        <v>826</v>
+      </c>
+      <c r="B16" s="0" t="s">
         <v>827</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>828</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
+        <v>829</v>
+      </c>
+      <c r="B18" s="0" t="s">
         <v>830</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>831</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
+        <v>832</v>
+      </c>
+      <c r="B20" s="0" t="s">
         <v>833</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>834</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
+        <v>834</v>
+      </c>
+      <c r="B21" s="0" t="s">
         <v>835</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>836</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
+        <v>836</v>
+      </c>
+      <c r="B22" s="0" t="s">
         <v>837</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>838</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
+        <v>838</v>
+      </c>
+      <c r="B23" s="0" t="s">
         <v>839</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>840</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
+        <v>840</v>
+      </c>
+      <c r="B24" s="0" t="s">
         <v>841</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>842</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
+        <v>842</v>
+      </c>
+      <c r="B25" s="0" t="s">
         <v>843</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>844</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
+        <v>844</v>
+      </c>
+      <c r="B26" s="0" t="s">
         <v>845</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>846</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
+        <v>846</v>
+      </c>
+      <c r="B27" s="0" t="s">
         <v>847</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>848</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
+        <v>848</v>
+      </c>
+      <c r="B28" s="0" t="s">
         <v>849</v>
-      </c>
-      <c r="B28" s="0" t="s">
-        <v>850</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
+        <v>850</v>
+      </c>
+      <c r="B29" s="0" t="s">
         <v>851</v>
-      </c>
-      <c r="B29" s="0" t="s">
-        <v>852</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>852</v>
+      </c>
+      <c r="B30" s="0" t="s">
         <v>853</v>
-      </c>
-      <c r="B30" s="0" t="s">
-        <v>854</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>854</v>
+      </c>
+      <c r="B31" s="0" t="s">
         <v>855</v>
-      </c>
-      <c r="B31" s="0" t="s">
-        <v>856</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>856</v>
+      </c>
+      <c r="B32" s="0" t="s">
         <v>857</v>
-      </c>
-      <c r="B32" s="0" t="s">
-        <v>858</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>858</v>
+      </c>
+      <c r="B33" s="0" t="s">
         <v>859</v>
-      </c>
-      <c r="B33" s="0" t="s">
-        <v>860</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>860</v>
+      </c>
+      <c r="B34" s="0" t="s">
         <v>861</v>
-      </c>
-      <c r="B34" s="0" t="s">
-        <v>862</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>862</v>
+      </c>
+      <c r="B35" s="0" t="s">
         <v>863</v>
-      </c>
-      <c r="B35" s="0" t="s">
-        <v>864</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
+        <v>864</v>
+      </c>
+      <c r="B36" s="0" t="s">
         <v>865</v>
-      </c>
-      <c r="B36" s="0" t="s">
-        <v>866</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
+        <v>866</v>
+      </c>
+      <c r="B37" s="0" t="s">
         <v>867</v>
-      </c>
-      <c r="B37" s="0" t="s">
-        <v>868</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
+        <v>868</v>
+      </c>
+      <c r="B38" s="0" t="s">
         <v>869</v>
-      </c>
-      <c r="B38" s="0" t="s">
-        <v>870</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
+        <v>870</v>
+      </c>
+      <c r="B39" s="0" t="s">
         <v>871</v>
-      </c>
-      <c r="B39" s="0" t="s">
-        <v>872</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
+        <v>872</v>
+      </c>
+      <c r="B40" s="0" t="s">
         <v>873</v>
-      </c>
-      <c r="B40" s="0" t="s">
-        <v>874</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
+        <v>874</v>
+      </c>
+      <c r="B41" s="0" t="s">
         <v>875</v>
-      </c>
-      <c r="B41" s="0" t="s">
-        <v>876</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
+        <v>877</v>
+      </c>
+      <c r="B43" s="0" t="s">
         <v>878</v>
-      </c>
-      <c r="B43" s="0" t="s">
-        <v>879</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
+        <v>879</v>
+      </c>
+      <c r="B44" s="0" t="s">
         <v>880</v>
-      </c>
-      <c r="B44" s="0" t="s">
-        <v>881</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
+        <v>881</v>
+      </c>
+      <c r="B45" s="0" t="s">
         <v>882</v>
-      </c>
-      <c r="B45" s="0" t="s">
-        <v>883</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
+        <v>883</v>
+      </c>
+      <c r="B46" s="0" t="s">
         <v>884</v>
-      </c>
-      <c r="B46" s="0" t="s">
-        <v>885</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
+        <v>885</v>
+      </c>
+      <c r="B47" s="0" t="s">
         <v>886</v>
-      </c>
-      <c r="B47" s="0" t="s">
-        <v>887</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
+        <v>887</v>
+      </c>
+      <c r="B48" s="0" t="s">
         <v>888</v>
-      </c>
-      <c r="B48" s="0" t="s">
-        <v>889</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
+        <v>890</v>
+      </c>
+      <c r="B50" s="0" t="s">
         <v>891</v>
-      </c>
-      <c r="B50" s="0" t="s">
-        <v>892</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
+        <v>892</v>
+      </c>
+      <c r="B51" s="0" t="s">
         <v>893</v>
-      </c>
-      <c r="B51" s="0" t="s">
-        <v>894</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
+        <v>894</v>
+      </c>
+      <c r="B52" s="0" t="s">
         <v>895</v>
-      </c>
-      <c r="B52" s="0" t="s">
-        <v>896</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -18625,22 +18649,22 @@
   </sheetPr>
   <dimension ref="A1:B112"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="E1:Z1 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="85.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="9.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>0</v>
       </c>
     </row>
@@ -18649,23 +18673,23 @@
         <v>37</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>897</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>898</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>899</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18673,7 +18697,7 @@
         <v>46</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18681,7 +18705,7 @@
         <v>50</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18689,7 +18713,7 @@
         <v>53</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18697,7 +18721,7 @@
         <v>57</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18705,7 +18729,7 @@
         <v>60</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18713,7 +18737,7 @@
         <v>64</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18721,7 +18745,7 @@
         <v>74</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18729,7 +18753,7 @@
         <v>82</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18737,7 +18761,7 @@
         <v>90</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18745,7 +18769,7 @@
         <v>93</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18753,7 +18777,7 @@
         <v>99</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18761,7 +18785,7 @@
         <v>104</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18769,7 +18793,7 @@
         <v>108</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18777,7 +18801,7 @@
         <v>112</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18785,7 +18809,7 @@
         <v>116</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18793,7 +18817,7 @@
         <v>126</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18801,7 +18825,7 @@
         <v>134</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18809,7 +18833,7 @@
         <v>143</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18817,7 +18841,7 @@
         <v>150</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18825,7 +18849,7 @@
         <v>157</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18833,7 +18857,7 @@
         <v>164</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18841,7 +18865,7 @@
         <v>171</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18849,7 +18873,7 @@
         <v>178</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18857,7 +18881,7 @@
         <v>184</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18865,7 +18889,7 @@
         <v>191</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18873,7 +18897,7 @@
         <v>197</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18881,7 +18905,7 @@
         <v>204</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18889,7 +18913,7 @@
         <v>207</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18897,7 +18921,7 @@
         <v>210</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18905,7 +18929,7 @@
         <v>214</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18913,7 +18937,7 @@
         <v>217</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18921,7 +18945,7 @@
         <v>220</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18929,7 +18953,7 @@
         <v>224</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18937,7 +18961,7 @@
         <v>227</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18945,7 +18969,7 @@
         <v>230</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18953,7 +18977,7 @@
         <v>234</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18961,7 +18985,7 @@
         <v>238</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18969,7 +18993,7 @@
         <v>242</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18977,7 +19001,7 @@
         <v>246</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18985,7 +19009,7 @@
         <v>250</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18993,7 +19017,7 @@
         <v>253</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19001,7 +19025,7 @@
         <v>257</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19009,7 +19033,7 @@
         <v>261</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19017,7 +19041,7 @@
         <v>271</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19025,7 +19049,7 @@
         <v>286</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19033,7 +19057,7 @@
         <v>290</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19041,7 +19065,7 @@
         <v>294</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19049,7 +19073,7 @@
         <v>298</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19057,7 +19081,7 @@
         <v>304</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19065,7 +19089,7 @@
         <v>308</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19073,7 +19097,7 @@
         <v>312</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19081,7 +19105,7 @@
         <v>317</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19089,7 +19113,7 @@
         <v>321</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19097,7 +19121,7 @@
         <v>325</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19105,7 +19129,7 @@
         <v>329</v>
       </c>
       <c r="B59" s="0" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19113,7 +19137,7 @@
         <v>333</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19121,7 +19145,7 @@
         <v>338</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19129,7 +19153,7 @@
         <v>342</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19137,7 +19161,7 @@
         <v>346</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19145,7 +19169,7 @@
         <v>350</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19153,7 +19177,7 @@
         <v>354</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19161,7 +19185,7 @@
         <v>358</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19169,7 +19193,7 @@
         <v>362</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19177,7 +19201,7 @@
         <v>366</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19185,7 +19209,7 @@
         <v>370</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19193,7 +19217,7 @@
         <v>374</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19201,7 +19225,7 @@
         <v>377</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19209,7 +19233,7 @@
         <v>380</v>
       </c>
       <c r="B72" s="0" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19217,7 +19241,7 @@
         <v>384</v>
       </c>
       <c r="B73" s="0" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19225,7 +19249,7 @@
         <v>387</v>
       </c>
       <c r="B74" s="0" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19233,7 +19257,7 @@
         <v>390</v>
       </c>
       <c r="B75" s="0" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19241,7 +19265,7 @@
         <v>395</v>
       </c>
       <c r="B76" s="0" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19249,7 +19273,7 @@
         <v>398</v>
       </c>
       <c r="B77" s="0" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19257,7 +19281,7 @@
         <v>404</v>
       </c>
       <c r="B78" s="0" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19265,7 +19289,7 @@
         <v>409</v>
       </c>
       <c r="B79" s="0" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19273,7 +19297,7 @@
         <v>412</v>
       </c>
       <c r="B80" s="0" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19281,7 +19305,7 @@
         <v>417</v>
       </c>
       <c r="B81" s="0" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19289,7 +19313,7 @@
         <v>422</v>
       </c>
       <c r="B82" s="0" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19297,7 +19321,7 @@
         <v>425</v>
       </c>
       <c r="B83" s="0" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19305,7 +19329,7 @@
         <v>429</v>
       </c>
       <c r="B84" s="0" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19313,7 +19337,7 @@
         <v>433</v>
       </c>
       <c r="B85" s="0" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19321,7 +19345,7 @@
         <v>437</v>
       </c>
       <c r="B86" s="0" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19329,7 +19353,7 @@
         <v>440</v>
       </c>
       <c r="B87" s="0" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19337,7 +19361,7 @@
         <v>443</v>
       </c>
       <c r="B88" s="0" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19345,7 +19369,7 @@
         <v>446</v>
       </c>
       <c r="B89" s="0" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19353,7 +19377,7 @@
         <v>449</v>
       </c>
       <c r="B90" s="0" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19361,7 +19385,7 @@
         <v>452</v>
       </c>
       <c r="B91" s="0" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19369,7 +19393,7 @@
         <v>455</v>
       </c>
       <c r="B92" s="0" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19377,7 +19401,7 @@
         <v>117</v>
       </c>
       <c r="B93" s="0" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19385,7 +19409,7 @@
         <v>127</v>
       </c>
       <c r="B94" s="0" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19393,7 +19417,7 @@
         <v>262</v>
       </c>
       <c r="B95" s="0" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19401,7 +19425,7 @@
         <v>264</v>
       </c>
       <c r="B96" s="0" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19409,7 +19433,7 @@
         <v>265</v>
       </c>
       <c r="B97" s="0" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19417,7 +19441,7 @@
         <v>266</v>
       </c>
       <c r="B98" s="0" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19425,7 +19449,7 @@
         <v>272</v>
       </c>
       <c r="B99" s="0" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19433,7 +19457,7 @@
         <v>273</v>
       </c>
       <c r="B100" s="0" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19441,7 +19465,7 @@
         <v>275</v>
       </c>
       <c r="B101" s="0" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19449,7 +19473,7 @@
         <v>277</v>
       </c>
       <c r="B102" s="0" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19457,7 +19481,7 @@
         <v>278</v>
       </c>
       <c r="B103" s="0" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19465,7 +19489,7 @@
         <v>279</v>
       </c>
       <c r="B104" s="0" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19473,7 +19497,7 @@
         <v>280</v>
       </c>
       <c r="B105" s="0" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19481,7 +19505,7 @@
         <v>399</v>
       </c>
       <c r="B106" s="0" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19489,7 +19513,7 @@
         <v>400</v>
       </c>
       <c r="B107" s="0" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19497,7 +19521,7 @@
         <v>523</v>
       </c>
       <c r="B108" s="0" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19505,7 +19529,7 @@
         <v>529</v>
       </c>
       <c r="B109" s="0" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19513,7 +19537,7 @@
         <v>534</v>
       </c>
       <c r="B110" s="0" t="s">
-        <v>1006</v>
+        <v>1005</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19521,7 +19545,7 @@
         <v>540</v>
       </c>
       <c r="B111" s="0" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19529,7 +19553,7 @@
         <v>546</v>
       </c>
       <c r="B112" s="0" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
     </row>
   </sheetData>

</xml_diff>